<commit_message>
shock and calc_all functions added to the new code
</commit_message>
<xml_diff>
--- a/CVX_Kenya/New Code/Shading_trees.xlsx
+++ b/CVX_Kenya/New Code/Shading_trees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\New Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A82E85C-BAED-4A48-94C2-208E674100B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910DA5E8-C48C-472F-80A0-C5A298373B2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13296" yWindow="2664" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -1669,7 +1669,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1809,7 +1809,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="0"/>
+        <f>G4</f>
         <v>0</v>
       </c>
       <c r="H5" s="2" t="s">

</xml_diff>

<commit_message>
merging calc_all and shock
into a single function named shock_calc
</commit_message>
<xml_diff>
--- a/CVX_Kenya/New Code/Shading_trees.xlsx
+++ b/CVX_Kenya/New Code/Shading_trees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\New Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910DA5E8-C48C-472F-80A0-C5A298373B2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFE9012-C351-4645-A98B-AAA0DCFE2817}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -1485,14 +1485,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="22.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9.109375" style="1"/>
@@ -1668,7 +1668,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new sensitivity function added
</commit_message>
<xml_diff>
--- a/CVX_Kenya/New Code/Shading_trees.xlsx
+++ b/CVX_Kenya/New Code/Shading_trees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\New Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E94A32-836E-48B1-AF77-9DAFD4554426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274D5743-25DC-4911-9F77-819189BB6E25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="271">
   <si>
     <t>level_row</t>
   </si>
@@ -867,12 +867,6 @@
   </si>
   <si>
     <t>ok</t>
-  </si>
-  <si>
-    <t>15-20</t>
-  </si>
-  <si>
-    <t>1800-2200</t>
   </si>
   <si>
     <t>aggregated</t>
@@ -1040,7 +1034,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1136,6 +1130,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1702,7 +1699,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -2041,7 +2038,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -2072,7 +2069,7 @@
         <v>9</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -2891,13 +2888,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C19" sqref="C19"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2906,14 +2903,14 @@
     <col min="2" max="2" width="74.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="186.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="5" max="8" width="14.5546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="186.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5546875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>175</v>
       </c>
@@ -2930,14 +2927,23 @@
         <v>220</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="I1" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="J1" s="10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="46" t="s">
         <v>181</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -2949,12 +2955,15 @@
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="45"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="46"/>
       <c r="B3" s="13" t="s">
         <v>247</v>
       </c>
@@ -2963,13 +2972,16 @@
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="11"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="11" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="11" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="45"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="46"/>
       <c r="B4" s="11" t="s">
         <v>183</v>
       </c>
@@ -2980,13 +2992,16 @@
         <v>248</v>
       </c>
       <c r="E4" s="11"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="11" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="46"/>
       <c r="B5" s="11" t="s">
         <v>216</v>
       </c>
@@ -2997,13 +3012,16 @@
         <v>219</v>
       </c>
       <c r="E5" s="11"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="11" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="45"/>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="46"/>
       <c r="B6" s="11" t="s">
         <v>217</v>
       </c>
@@ -3011,14 +3029,23 @@
         <v>2000</v>
       </c>
       <c r="D6" s="12"/>
-      <c r="E6" s="11" t="s">
-        <v>271</v>
-      </c>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="45"/>
+      <c r="E6" s="44" t="s">
+        <v>205</v>
+      </c>
+      <c r="F6" s="44">
+        <v>1800</v>
+      </c>
+      <c r="G6" s="44">
+        <v>2200</v>
+      </c>
+      <c r="H6" s="44">
+        <v>100</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="46"/>
       <c r="B7" s="11" t="s">
         <v>188</v>
       </c>
@@ -3029,14 +3056,17 @@
         <v>187</v>
       </c>
       <c r="E7" s="11"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="26" t="s">
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="26" t="s">
         <v>192</v>
       </c>
-      <c r="H7" s="25"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="45"/>
+      <c r="K7" s="25"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="46"/>
       <c r="B8" s="11" t="s">
         <v>241</v>
       </c>
@@ -3047,16 +3077,25 @@
         <v>244</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="F8" s="12"/>
-      <c r="G8" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="F8" s="11">
+        <v>15</v>
+      </c>
+      <c r="G8" s="11">
+        <v>20</v>
+      </c>
+      <c r="H8" s="11">
+        <v>1</v>
+      </c>
+      <c r="I8" s="12"/>
+      <c r="J8" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="H8" s="25"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="45"/>
+      <c r="K8" s="25"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="46"/>
       <c r="B9" s="11" t="s">
         <v>240</v>
       </c>
@@ -3067,14 +3106,17 @@
         <v>245</v>
       </c>
       <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="26" t="s">
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="26" t="s">
         <v>246</v>
       </c>
-      <c r="H9" s="25"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="45"/>
+      <c r="K9" s="25"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="46"/>
       <c r="B10" s="11" t="s">
         <v>243</v>
       </c>
@@ -3085,13 +3127,16 @@
         <v>190</v>
       </c>
       <c r="E10" s="12"/>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="G10" s="11"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="45"/>
+      <c r="J10" s="11"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="46"/>
       <c r="B11" s="11" t="s">
         <v>193</v>
       </c>
@@ -3099,14 +3144,17 @@
         <v>1.4</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="11"/>
+      <c r="F11" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="45"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="46"/>
       <c r="B12" s="11" t="s">
         <v>194</v>
       </c>
@@ -3114,14 +3162,17 @@
         <v>1.4</v>
       </c>
       <c r="D12" s="11"/>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="11"/>
+      <c r="F12" s="11" t="s">
         <v>266</v>
       </c>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="45"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="46"/>
       <c r="B13" s="13" t="s">
         <v>182</v>
       </c>
@@ -3131,12 +3182,15 @@
       <c r="D13" s="13"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
-      <c r="G13" s="13" t="s">
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="45"/>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="46"/>
       <c r="B14" s="13" t="s">
         <v>200</v>
       </c>
@@ -3147,8 +3201,11 @@
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="38"/>
       <c r="B15" s="13" t="s">
         <v>250</v>
@@ -3157,15 +3214,18 @@
         <v>-0.08</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="13"/>
+      <c r="F15" s="13" t="s">
         <v>267</v>
       </c>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13" t="s">
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="38"/>
       <c r="B16" s="13" t="s">
         <v>251</v>
@@ -3177,8 +3237,11 @@
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="40"/>
       <c r="B17" s="13" t="s">
         <v>254</v>
@@ -3189,12 +3252,15 @@
       <c r="D17" s="13"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="44" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="45" t="s">
         <v>184</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -3207,9 +3273,12 @@
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="44"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="45"/>
       <c r="B19" s="14" t="s">
         <v>189</v>
       </c>
@@ -3217,18 +3286,21 @@
         <v>1.4E-2</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="14"/>
+      <c r="F19" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="J19" s="14" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="44"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="45"/>
       <c r="B20" s="14" t="s">
         <v>195</v>
       </c>
@@ -3238,15 +3310,18 @@
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="J20" s="14" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="44"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="45"/>
       <c r="B21" s="14" t="s">
         <v>196</v>
       </c>
@@ -3256,14 +3331,17 @@
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
-      <c r="F21" s="14" t="s">
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="G21" s="14" t="s">
+      <c r="J21" s="14" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="39"/>
       <c r="B22" s="14" t="s">
         <v>257</v>
@@ -3275,8 +3353,11 @@
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="14"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="29" t="s">
         <v>177</v>
       </c>
@@ -3293,8 +3374,11 @@
       <c r="E23" s="17"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="29"/>
       <c r="B24" s="16" t="s">
         <v>185</v>
@@ -3307,13 +3391,16 @@
         <v>190</v>
       </c>
       <c r="E24" s="16"/>
-      <c r="F24" s="16" t="s">
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16" t="s">
         <v>203</v>
       </c>
-      <c r="G24" s="17"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="46"/>
+      <c r="J24" s="17"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="47"/>
       <c r="B25" s="15" t="s">
         <v>252</v>
       </c>
@@ -3323,15 +3410,18 @@
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="15"/>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="J25" s="15" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="46"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="47"/>
       <c r="B26" s="15" t="s">
         <v>201</v>
       </c>
@@ -3341,13 +3431,16 @@
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="15"/>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="G26" s="15"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="46"/>
+      <c r="J26" s="15"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="47"/>
       <c r="B27" s="15" t="s">
         <v>202</v>
       </c>
@@ -3357,12 +3450,15 @@
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="15"/>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="J27" s="15"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="41"/>
       <c r="B28" s="15" t="s">
         <v>202</v>
@@ -3375,9 +3471,12 @@
       <c r="E28" s="15"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="47" t="s">
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="48" t="s">
         <v>224</v>
       </c>
       <c r="B29" s="31" t="s">
@@ -3391,13 +3490,16 @@
         <v>190</v>
       </c>
       <c r="E29" s="31"/>
-      <c r="F29" s="31" t="s">
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31" t="s">
         <v>198</v>
       </c>
-      <c r="G29" s="31"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="47"/>
+      <c r="J29" s="31"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="48"/>
       <c r="B30" s="31" t="s">
         <v>252</v>
       </c>
@@ -3407,15 +3509,18 @@
       </c>
       <c r="D30" s="31"/>
       <c r="E30" s="31"/>
-      <c r="F30" s="31" t="s">
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="J30" s="31" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="47"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="48"/>
       <c r="B31" s="31" t="s">
         <v>225</v>
       </c>
@@ -3424,15 +3529,18 @@
       </c>
       <c r="D31" s="31"/>
       <c r="E31" s="31"/>
-      <c r="F31" s="31" t="s">
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="G31" s="31" t="s">
+      <c r="J31" s="31" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="47"/>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="48"/>
       <c r="B32" s="31" t="s">
         <v>226</v>
       </c>
@@ -3442,14 +3550,17 @@
       </c>
       <c r="D32" s="31"/>
       <c r="E32" s="31"/>
-      <c r="F32" s="31" t="s">
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="J32" s="31" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B33" s="31" t="s">
         <v>253</v>
       </c>
@@ -3459,14 +3570,17 @@
       </c>
       <c r="D33" s="31"/>
       <c r="E33" s="31"/>
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31" t="s">
         <v>136</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="J33" s="31" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B34" s="31" t="s">
         <v>242</v>
       </c>
@@ -3476,14 +3590,17 @@
       </c>
       <c r="D34" s="31"/>
       <c r="E34" s="31"/>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="J34" s="31" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B35" s="31" t="s">
         <v>255</v>
       </c>
@@ -3493,14 +3610,17 @@
       </c>
       <c r="D35" s="31"/>
       <c r="E35" s="31"/>
-      <c r="F35" s="31" t="s">
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="J35" s="31" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>249</v>
       </c>
@@ -3513,7 +3633,7 @@
     <mergeCell ref="A29:A32"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G7" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="J7" r:id="rId1" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
price ration plot function added
</commit_message>
<xml_diff>
--- a/CVX_Kenya/New Code/Shading_trees.xlsx
+++ b/CVX_Kenya/New Code/Shading_trees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\New Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{658B6B15-32AB-4824-ACD9-F7731BFDA966}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3494BBEC-7CD9-45D3-9CEE-28E857E5F881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="S" sheetId="7" r:id="rId1"/>
@@ -1034,7 +1034,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1144,6 +1144,30 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1662,7 +1686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -2644,11 +2668,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2657,7 +2681,8 @@
     <col min="2" max="2" width="74.5546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="14.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" style="2" customWidth="1"/>
+    <col min="6" max="8" width="14.5546875" style="1" customWidth="1"/>
     <col min="9" max="9" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="186.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.5546875" style="1" customWidth="1"/>
@@ -2677,7 +2702,7 @@
       <c r="D1" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="49" t="s">
         <v>220</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -2707,7 +2732,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
+      <c r="E2" s="50"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -2725,7 +2750,7 @@
         <v>0.25</v>
       </c>
       <c r="D3" s="12"/>
-      <c r="E3" s="11"/>
+      <c r="E3" s="44"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
       <c r="H3" s="11"/>
@@ -2745,7 +2770,7 @@
       <c r="D4" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="E4" s="11"/>
+      <c r="E4" s="44"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -2765,7 +2790,7 @@
       <c r="D5" s="11" t="s">
         <v>219</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="44"/>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -2786,13 +2811,13 @@
       <c r="E6" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="F6" s="44">
+      <c r="F6" s="56">
         <v>1800</v>
       </c>
-      <c r="G6" s="44">
+      <c r="G6" s="56">
         <v>2200</v>
       </c>
-      <c r="H6" s="44">
+      <c r="H6" s="56">
         <v>100</v>
       </c>
       <c r="I6" s="12"/>
@@ -2809,10 +2834,10 @@
       <c r="D7" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="56"/>
+      <c r="H7" s="56"/>
       <c r="I7" s="12"/>
       <c r="J7" s="26" t="s">
         <v>192</v>
@@ -2830,16 +2855,16 @@
       <c r="D8" s="11" t="s">
         <v>244</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="56">
         <v>15</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="56">
         <v>20</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="56">
         <v>1</v>
       </c>
       <c r="I8" s="12"/>
@@ -2859,10 +2884,10 @@
       <c r="D9" s="11" t="s">
         <v>245</v>
       </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
+      <c r="E9" s="44"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="56"/>
+      <c r="H9" s="56"/>
       <c r="I9" s="12"/>
       <c r="J9" s="26" t="s">
         <v>246</v>
@@ -2880,7 +2905,7 @@
       <c r="D10" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" s="50"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -2898,7 +2923,7 @@
         <v>1.4</v>
       </c>
       <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="E11" s="44"/>
       <c r="F11" s="11" t="s">
         <v>266</v>
       </c>
@@ -2916,7 +2941,7 @@
         <v>1.4</v>
       </c>
       <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
+      <c r="E12" s="44"/>
       <c r="F12" s="11" t="s">
         <v>266</v>
       </c>
@@ -2934,7 +2959,7 @@
         <v>800000</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
+      <c r="E13" s="51"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -2952,7 +2977,7 @@
         <v>8.3479305095333606E-2</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="E14" s="51"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
@@ -2968,7 +2993,7 @@
         <v>-0.08</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
+      <c r="E15" s="51"/>
       <c r="F15" s="13" t="s">
         <v>267</v>
       </c>
@@ -2988,7 +3013,7 @@
         <v>-0.02</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
+      <c r="E16" s="51"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -3004,7 +3029,7 @@
         <v>3.8</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
+      <c r="E17" s="51"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
@@ -3024,7 +3049,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
+      <c r="E18" s="52"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -3040,7 +3065,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
+      <c r="E19" s="52"/>
       <c r="F19" s="14" t="s">
         <v>268</v>
       </c>
@@ -3063,7 +3088,7 @@
         <v>-0.39999999999999991</v>
       </c>
       <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
+      <c r="E20" s="52"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -3084,7 +3109,7 @@
         <v>-0.39999999999999991</v>
       </c>
       <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
+      <c r="E21" s="52"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -3104,7 +3129,7 @@
         <v>-0.4</v>
       </c>
       <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+      <c r="E22" s="52"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -3125,7 +3150,7 @@
       <c r="D23" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="E23" s="17"/>
+      <c r="E23" s="53"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
@@ -3144,7 +3169,7 @@
       <c r="D24" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="E24" s="16"/>
+      <c r="E24" s="53"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
@@ -3163,7 +3188,7 @@
         <v>-0.02</v>
       </c>
       <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+      <c r="E25" s="54"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -3184,7 +3209,7 @@
         <v>-3.3391722038133433E-2</v>
       </c>
       <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
+      <c r="E26" s="54"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -3203,7 +3228,7 @@
         <v>-3.3391722038133433E-2</v>
       </c>
       <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
+      <c r="E27" s="54"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -3222,7 +3247,7 @@
         <v>-3.3391722038133446E-2</v>
       </c>
       <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
+      <c r="E28" s="54"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
@@ -3243,7 +3268,7 @@
       <c r="D29" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="E29" s="31"/>
+      <c r="E29" s="55"/>
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
@@ -3262,7 +3287,7 @@
         <v>-0.02</v>
       </c>
       <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
+      <c r="E30" s="55"/>
       <c r="F30" s="31"/>
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
@@ -3282,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
+      <c r="E31" s="55"/>
       <c r="F31" s="31"/>
       <c r="G31" s="31"/>
       <c r="H31" s="31"/>
@@ -3303,7 +3328,7 @@
         <v>-2.2539412375740076E-2</v>
       </c>
       <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
+      <c r="E32" s="55"/>
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
       <c r="H32" s="31"/>
@@ -3323,7 +3348,7 @@
         <v>3.1722135936226768E-2</v>
       </c>
       <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
+      <c r="E33" s="55"/>
       <c r="F33" s="31"/>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
@@ -3343,7 +3368,7 @@
         <v>-0.44520605187319889</v>
       </c>
       <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
+      <c r="E34" s="55"/>
       <c r="F34" s="31"/>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -3363,7 +3388,7 @@
         <v>-335.45639999999997</v>
       </c>
       <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
+      <c r="E35" s="55"/>
       <c r="F35" s="31"/>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>

</xml_diff>

<commit_message>
impact assessment implemented but not working properly
the way taht the shock in the module is implemented is not right
</commit_message>
<xml_diff>
--- a/CVX_Kenya/New Code/Shading_trees.xlsx
+++ b/CVX_Kenya/New Code/Shading_trees.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\payam\Documents\GitHub\CIVICS_Kenya\CVX_Kenya\New Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3494BBEC-7CD9-45D3-9CEE-28E857E5F881}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1C201C-FF6B-4939-85F4-091D101636CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1134,6 +1134,30 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1144,30 +1168,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1575,7 +1575,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2672,7 +2672,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2702,7 +2702,7 @@
       <c r="D1" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="45" t="s">
         <v>220</v>
       </c>
       <c r="F1" s="10" t="s">
@@ -2722,7 +2722,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="54" t="s">
         <v>181</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -2732,7 +2732,7 @@
         <v>0.5</v>
       </c>
       <c r="D2" s="12"/>
-      <c r="E2" s="50"/>
+      <c r="E2" s="46"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -2742,7 +2742,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="46"/>
+      <c r="A3" s="54"/>
       <c r="B3" s="13" t="s">
         <v>247</v>
       </c>
@@ -2760,7 +2760,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="46"/>
+      <c r="A4" s="54"/>
       <c r="B4" s="11" t="s">
         <v>183</v>
       </c>
@@ -2780,7 +2780,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="46"/>
+      <c r="A5" s="54"/>
       <c r="B5" s="11" t="s">
         <v>216</v>
       </c>
@@ -2800,7 +2800,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="46"/>
+      <c r="A6" s="54"/>
       <c r="B6" s="11" t="s">
         <v>217</v>
       </c>
@@ -2811,20 +2811,20 @@
       <c r="E6" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="F6" s="56">
+      <c r="F6" s="52">
         <v>1800</v>
       </c>
-      <c r="G6" s="56">
+      <c r="G6" s="52">
         <v>2200</v>
       </c>
-      <c r="H6" s="56">
+      <c r="H6" s="52">
         <v>100</v>
       </c>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="46"/>
+      <c r="A7" s="54"/>
       <c r="B7" s="11" t="s">
         <v>188</v>
       </c>
@@ -2835,9 +2835,9 @@
         <v>187</v>
       </c>
       <c r="E7" s="44"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
-      <c r="H7" s="56"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
       <c r="I7" s="12"/>
       <c r="J7" s="26" t="s">
         <v>192</v>
@@ -2845,7 +2845,7 @@
       <c r="K7" s="25"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="46"/>
+      <c r="A8" s="54"/>
       <c r="B8" s="11" t="s">
         <v>241</v>
       </c>
@@ -2858,13 +2858,13 @@
       <c r="E8" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="F8" s="56">
+      <c r="F8" s="52">
         <v>15</v>
       </c>
-      <c r="G8" s="56">
+      <c r="G8" s="52">
         <v>20</v>
       </c>
-      <c r="H8" s="56">
+      <c r="H8" s="52">
         <v>1</v>
       </c>
       <c r="I8" s="12"/>
@@ -2874,7 +2874,7 @@
       <c r="K8" s="25"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="46"/>
+      <c r="A9" s="54"/>
       <c r="B9" s="11" t="s">
         <v>240</v>
       </c>
@@ -2885,9 +2885,9 @@
         <v>245</v>
       </c>
       <c r="E9" s="44"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
       <c r="I9" s="12"/>
       <c r="J9" s="26" t="s">
         <v>246</v>
@@ -2895,7 +2895,7 @@
       <c r="K9" s="25"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="46"/>
+      <c r="A10" s="54"/>
       <c r="B10" s="11" t="s">
         <v>243</v>
       </c>
@@ -2905,7 +2905,7 @@
       <c r="D10" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="E10" s="50"/>
+      <c r="E10" s="46"/>
       <c r="F10" s="12"/>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
@@ -2915,7 +2915,7 @@
       <c r="J10" s="11"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="46"/>
+      <c r="A11" s="54"/>
       <c r="B11" s="11" t="s">
         <v>193</v>
       </c>
@@ -2933,7 +2933,7 @@
       <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="46"/>
+      <c r="A12" s="54"/>
       <c r="B12" s="11" t="s">
         <v>194</v>
       </c>
@@ -2951,7 +2951,7 @@
       <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="46"/>
+      <c r="A13" s="54"/>
       <c r="B13" s="13" t="s">
         <v>182</v>
       </c>
@@ -2959,7 +2959,7 @@
         <v>800000</v>
       </c>
       <c r="D13" s="13"/>
-      <c r="E13" s="51"/>
+      <c r="E13" s="47"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
       <c r="H13" s="13"/>
@@ -2969,7 +2969,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="46"/>
+      <c r="A14" s="54"/>
       <c r="B14" s="13" t="s">
         <v>200</v>
       </c>
@@ -2977,7 +2977,7 @@
         <v>8.3479305095333606E-2</v>
       </c>
       <c r="D14" s="13"/>
-      <c r="E14" s="51"/>
+      <c r="E14" s="47"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
       <c r="H14" s="13"/>
@@ -2993,7 +2993,7 @@
         <v>-0.08</v>
       </c>
       <c r="D15" s="13"/>
-      <c r="E15" s="51"/>
+      <c r="E15" s="47"/>
       <c r="F15" s="13" t="s">
         <v>267</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>-0.02</v>
       </c>
       <c r="D16" s="13"/>
-      <c r="E16" s="51"/>
+      <c r="E16" s="47"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
       <c r="H16" s="13"/>
@@ -3029,7 +3029,7 @@
         <v>3.8</v>
       </c>
       <c r="D17" s="13"/>
-      <c r="E17" s="51"/>
+      <c r="E17" s="47"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
@@ -3039,7 +3039,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="45" t="s">
+      <c r="A18" s="53" t="s">
         <v>184</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -3049,7 +3049,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="14"/>
-      <c r="E18" s="52"/>
+      <c r="E18" s="48"/>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -3057,7 +3057,7 @@
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="45"/>
+      <c r="A19" s="53"/>
       <c r="B19" s="14" t="s">
         <v>189</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>1.4E-2</v>
       </c>
       <c r="D19" s="14"/>
-      <c r="E19" s="52"/>
+      <c r="E19" s="48"/>
       <c r="F19" s="14" t="s">
         <v>268</v>
       </c>
@@ -3079,7 +3079,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="45"/>
+      <c r="A20" s="53"/>
       <c r="B20" s="14" t="s">
         <v>195</v>
       </c>
@@ -3088,7 +3088,7 @@
         <v>-0.39999999999999991</v>
       </c>
       <c r="D20" s="14"/>
-      <c r="E20" s="52"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -3100,7 +3100,7 @@
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="45"/>
+      <c r="A21" s="53"/>
       <c r="B21" s="14" t="s">
         <v>196</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>-0.39999999999999991</v>
       </c>
       <c r="D21" s="14"/>
-      <c r="E21" s="52"/>
+      <c r="E21" s="48"/>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
@@ -3129,7 +3129,7 @@
         <v>-0.4</v>
       </c>
       <c r="D22" s="14"/>
-      <c r="E22" s="52"/>
+      <c r="E22" s="48"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -3150,7 +3150,7 @@
       <c r="D23" s="17" t="s">
         <v>190</v>
       </c>
-      <c r="E23" s="53"/>
+      <c r="E23" s="49"/>
       <c r="F23" s="17"/>
       <c r="G23" s="17"/>
       <c r="H23" s="17"/>
@@ -3169,7 +3169,7 @@
       <c r="D24" s="16" t="s">
         <v>190</v>
       </c>
-      <c r="E24" s="53"/>
+      <c r="E24" s="49"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
@@ -3179,7 +3179,7 @@
       <c r="J24" s="17"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="47"/>
+      <c r="A25" s="55"/>
       <c r="B25" s="15" t="s">
         <v>252</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>-0.02</v>
       </c>
       <c r="D25" s="15"/>
-      <c r="E25" s="54"/>
+      <c r="E25" s="50"/>
       <c r="F25" s="15"/>
       <c r="G25" s="15"/>
       <c r="H25" s="15"/>
@@ -3200,7 +3200,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="47"/>
+      <c r="A26" s="55"/>
       <c r="B26" s="15" t="s">
         <v>201</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>-3.3391722038133433E-2</v>
       </c>
       <c r="D26" s="15"/>
-      <c r="E26" s="54"/>
+      <c r="E26" s="50"/>
       <c r="F26" s="15"/>
       <c r="G26" s="15"/>
       <c r="H26" s="15"/>
@@ -3219,7 +3219,7 @@
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="47"/>
+      <c r="A27" s="55"/>
       <c r="B27" s="15" t="s">
         <v>202</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>-3.3391722038133433E-2</v>
       </c>
       <c r="D27" s="15"/>
-      <c r="E27" s="54"/>
+      <c r="E27" s="50"/>
       <c r="F27" s="15"/>
       <c r="G27" s="15"/>
       <c r="H27" s="15"/>
@@ -3247,7 +3247,7 @@
         <v>-3.3391722038133446E-2</v>
       </c>
       <c r="D28" s="15"/>
-      <c r="E28" s="54"/>
+      <c r="E28" s="50"/>
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
       <c r="H28" s="15"/>
@@ -3255,7 +3255,7 @@
       <c r="J28" s="15"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="56" t="s">
         <v>224</v>
       </c>
       <c r="B29" s="31" t="s">
@@ -3268,7 +3268,7 @@
       <c r="D29" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="E29" s="55"/>
+      <c r="E29" s="51"/>
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
       <c r="H29" s="31"/>
@@ -3278,7 +3278,7 @@
       <c r="J29" s="31"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A30" s="48"/>
+      <c r="A30" s="56"/>
       <c r="B30" s="31" t="s">
         <v>252</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>-0.02</v>
       </c>
       <c r="D30" s="31"/>
-      <c r="E30" s="55"/>
+      <c r="E30" s="51"/>
       <c r="F30" s="31"/>
       <c r="G30" s="31"/>
       <c r="H30" s="31"/>
@@ -3299,7 +3299,7 @@
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A31" s="48"/>
+      <c r="A31" s="56"/>
       <c r="B31" s="31" t="s">
         <v>225</v>
       </c>
@@ -3307,7 +3307,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="31"/>
-      <c r="E31" s="55"/>
+      <c r="E31" s="51"/>
       <c r="F31" s="31"/>
       <c r="G31" s="31"/>
       <c r="H31" s="31"/>
@@ -3319,7 +3319,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A32" s="48"/>
+      <c r="A32" s="56"/>
       <c r="B32" s="31" t="s">
         <v>226</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>-2.2539412375740076E-2</v>
       </c>
       <c r="D32" s="31"/>
-      <c r="E32" s="55"/>
+      <c r="E32" s="51"/>
       <c r="F32" s="31"/>
       <c r="G32" s="31"/>
       <c r="H32" s="31"/>
@@ -3348,7 +3348,7 @@
         <v>3.1722135936226768E-2</v>
       </c>
       <c r="D33" s="31"/>
-      <c r="E33" s="55"/>
+      <c r="E33" s="51"/>
       <c r="F33" s="31"/>
       <c r="G33" s="31"/>
       <c r="H33" s="31"/>
@@ -3368,7 +3368,7 @@
         <v>-0.44520605187319889</v>
       </c>
       <c r="D34" s="31"/>
-      <c r="E34" s="55"/>
+      <c r="E34" s="51"/>
       <c r="F34" s="31"/>
       <c r="G34" s="31"/>
       <c r="H34" s="31"/>
@@ -3388,7 +3388,7 @@
         <v>-335.45639999999997</v>
       </c>
       <c r="D35" s="31"/>
-      <c r="E35" s="55"/>
+      <c r="E35" s="51"/>
       <c r="F35" s="31"/>
       <c r="G35" s="31"/>
       <c r="H35" s="31"/>

</xml_diff>